<commit_message>
Mejoras en generación de actas Información de grupos en pantalla Generacion de fase final
</commit_message>
<xml_diff>
--- a/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/actaVPJuegosDeportivos.xlsx
+++ b/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/actaVPJuegosDeportivos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\srcRepository\Proyectos Estela\Federacion\VoleyPlaya.GestionWeb\wwwroot\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D0D3AF-A3E9-40ED-B15B-3F107442649A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB9B4A1-96BE-4821-AFC2-69516AF44A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{85829934-520D-40B5-91EB-5AB354E166AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85829934-520D-40B5-91EB-5AB354E166AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Acta" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>ACTA DE VOLEY PLAYA</t>
   </si>
@@ -73,12 +73,15 @@
   <si>
     <t>Comité Asturiano de Árbitros</t>
   </si>
+  <si>
+    <t>RONDA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +138,14 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -247,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -275,6 +286,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -284,13 +298,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2059,8 +2073,8 @@
   </sheetPr>
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42:I42"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2090,25 +2104,25 @@
       <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="22"/>
     </row>
     <row r="3" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="4"/>
@@ -2119,14 +2133,15 @@
       <c r="Q3" s="7"/>
     </row>
     <row r="4" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
       <c r="L4" s="5"/>
       <c r="N4" s="6" t="s">
         <v>1</v>
@@ -2138,7 +2153,7 @@
       <c r="A5" s="4"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="4"/>
       <c r="D6" s="9" t="s">
         <v>2</v>
@@ -2157,6 +2172,10 @@
       </c>
       <c r="L6" s="23"/>
       <c r="M6" s="23"/>
+      <c r="N6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" s="8"/>
       <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -2190,8 +2209,10 @@
       <c r="M9" s="24"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
+      <c r="E10" s="25"/>
+      <c r="K10" s="25"/>
       <c r="Q10" s="7"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -2320,10 +2341,10 @@
     </row>
     <row r="42" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="4"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
       <c r="Q42" s="7"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -2378,8 +2399,8 @@
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="G4:H4"/>
     <mergeCell ref="J4:K4"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>